<commit_message>
Updated data to fix month issues in species sheet
</commit_message>
<xml_diff>
--- a/data-raw/mCRM_bird_parameter_Defaults v2.0.xlsx
+++ b/data-raw/mCRM_bird_parameter_Defaults v2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HC0054 - MSS update to sCRM\300 - Technical\mCRM\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D38B1DA-8ED9-4BD7-B79B-718D76F54559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B698C9-0378-4AFE-AB60-3EEEF058B35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="2490" windowWidth="17265" windowHeight="9660" xr2:uid="{1C3AA158-F65C-4955-A6B9-80286CA44754}"/>
+    <workbookView xWindow="2715" yWindow="1905" windowWidth="20010" windowHeight="14010" xr2:uid="{1C3AA158-F65C-4955-A6B9-80286CA44754}"/>
   </bookViews>
   <sheets>
     <sheet name="Default Values" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="287">
   <si>
     <t>Body_length</t>
   </si>
@@ -862,16 +862,7 @@
     <t>june,july</t>
   </si>
   <si>
-    <t>August,september,october,november,december</t>
-  </si>
-  <si>
     <t>july,august,september,october,november,december</t>
-  </si>
-  <si>
-    <t>june,july,august, september</t>
-  </si>
-  <si>
-    <t>june,july,august,september, october</t>
   </si>
   <si>
     <t>gr_whfgo</t>
@@ -1289,10 +1280,10 @@
   <dimension ref="A1:T71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="O17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,7 +1301,7 @@
     <col min="12" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="49" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.5703125" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -1394,7 +1385,7 @@
         <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F2">
         <v>1.52</v>
@@ -1630,7 +1621,7 @@
         <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F6">
         <v>0.72</v>
@@ -1689,7 +1680,7 @@
         <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F7">
         <v>0.72</v>
@@ -1807,7 +1798,7 @@
         <v>101</v>
       </c>
       <c r="E9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F9">
         <v>0.64</v>
@@ -1866,7 +1857,7 @@
         <v>101</v>
       </c>
       <c r="E10" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F10">
         <v>0.64</v>
@@ -1925,7 +1916,7 @@
         <v>102</v>
       </c>
       <c r="E11" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F11">
         <v>0.57999999999999996</v>
@@ -1984,7 +1975,7 @@
         <v>102</v>
       </c>
       <c r="E12" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F12">
         <v>0.57999999999999996</v>
@@ -2043,7 +2034,7 @@
         <v>103</v>
       </c>
       <c r="E13" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F13">
         <v>0.57999999999999996</v>
@@ -2135,7 +2126,7 @@
         <v>274</v>
       </c>
       <c r="P14" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="Q14">
         <v>0.98499999999999999</v>
@@ -2282,7 +2273,7 @@
         <v>116</v>
       </c>
       <c r="E17" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F17">
         <v>0.36</v>
@@ -2312,7 +2303,7 @@
         <v>257</v>
       </c>
       <c r="O17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Q17">
         <v>0.98499999999999999</v>
@@ -3085,7 +3076,7 @@
         <v>239</v>
       </c>
       <c r="O30" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="Q30">
         <v>0.98499999999999999</v>
@@ -3409,7 +3400,7 @@
         <v>155</v>
       </c>
       <c r="E36" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F36">
         <v>0.24</v>
@@ -3645,7 +3636,7 @@
         <v>161</v>
       </c>
       <c r="E40" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F40">
         <v>0.25</v>
@@ -3973,7 +3964,7 @@
         <v>239</v>
       </c>
       <c r="O45" t="s">
-        <v>278</v>
+        <v>247</v>
       </c>
       <c r="Q45">
         <v>0.999</v>

</xml_diff>